<commit_message>
GoodInfo_v2 - 2021-12-29 完成
</commit_message>
<xml_diff>
--- a/StockList_2021-12-29.xlsx
+++ b/StockList_2021-12-29.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ray\Documents\Python\GoodInfo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RayWu\OneDrive - AAEON Technology\_OLD\Documents\Python\GoodInfo_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_A966A992F95B6A23BFDC323B86F3FA90A1A35C63" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{EE0E07A9-1F0A-45FB-9E30-2D17651F875A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11856"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11856" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AQ$293</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1875" uniqueCount="1053">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1882" uniqueCount="1051">
   <si>
     <t>代號</t>
   </si>
@@ -3188,22 +3189,14 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>v</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
+    <t>o</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3262,11 +3255,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -3568,11 +3562,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AQ293"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W154" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AE163" sqref="AE163"/>
+    <sheetView tabSelected="1" topLeftCell="W155" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AL179" activeCellId="4" sqref="AL158 AL161 AL162 AL172 AL179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -18599,10 +18593,10 @@
       <c r="AD157" t="s">
         <v>119</v>
       </c>
-      <c r="AE157">
-        <v>1</v>
-      </c>
-      <c r="AF157">
+      <c r="AE157" t="s">
+        <v>1049</v>
+      </c>
+      <c r="AF157" s="2">
         <v>3</v>
       </c>
       <c r="AG157" t="s">
@@ -18718,11 +18712,11 @@
       <c r="AD158" t="s">
         <v>179</v>
       </c>
-      <c r="AE158" t="s">
-        <v>1049</v>
-      </c>
-      <c r="AF158">
-        <v>3</v>
+      <c r="AE158">
+        <v>1</v>
+      </c>
+      <c r="AF158" s="2">
+        <v>2.9</v>
       </c>
       <c r="AG158" t="s">
         <v>180</v>
@@ -18849,7 +18843,7 @@
       <c r="AE159">
         <v>1</v>
       </c>
-      <c r="AF159">
+      <c r="AF159" s="2">
         <v>3</v>
       </c>
       <c r="AG159" t="s">
@@ -18966,9 +18960,9 @@
         <v>274</v>
       </c>
       <c r="AE160" t="s">
-        <v>1050</v>
-      </c>
-      <c r="AF160">
+        <v>1049</v>
+      </c>
+      <c r="AF160" s="2">
         <v>3</v>
       </c>
       <c r="AG160" t="s">
@@ -19084,11 +19078,11 @@
       <c r="AD161" t="s">
         <v>424</v>
       </c>
-      <c r="AE161" t="s">
-        <v>1051</v>
-      </c>
-      <c r="AF161">
-        <v>3</v>
+      <c r="AE161">
+        <v>1</v>
+      </c>
+      <c r="AF161" s="2">
+        <v>2.8</v>
       </c>
       <c r="AG161" t="s">
         <v>425</v>
@@ -19212,10 +19206,10 @@
       <c r="AD162" t="s">
         <v>434</v>
       </c>
-      <c r="AE162" t="s">
-        <v>1052</v>
-      </c>
-      <c r="AF162">
+      <c r="AE162">
+        <v>1</v>
+      </c>
+      <c r="AF162" s="2">
         <v>3</v>
       </c>
       <c r="AG162" t="s">
@@ -19343,7 +19337,7 @@
       <c r="AE163">
         <v>1</v>
       </c>
-      <c r="AF163">
+      <c r="AF163" s="2">
         <v>3</v>
       </c>
       <c r="AG163" t="s">
@@ -19459,10 +19453,10 @@
       <c r="AD164" t="s">
         <v>648</v>
       </c>
-      <c r="AE164">
-        <v>1</v>
-      </c>
-      <c r="AF164">
+      <c r="AE164" t="s">
+        <v>1049</v>
+      </c>
+      <c r="AF164" s="2">
         <v>3</v>
       </c>
       <c r="AG164" t="s">
@@ -19578,10 +19572,10 @@
       <c r="AD165" t="s">
         <v>733</v>
       </c>
-      <c r="AE165">
-        <v>1</v>
-      </c>
-      <c r="AF165">
+      <c r="AE165" t="s">
+        <v>1050</v>
+      </c>
+      <c r="AF165" s="2">
         <v>3</v>
       </c>
       <c r="AG165" t="s">
@@ -19703,7 +19697,7 @@
       <c r="AE166">
         <v>1</v>
       </c>
-      <c r="AF166">
+      <c r="AF166" s="2">
         <v>3</v>
       </c>
       <c r="AG166" t="s">
@@ -19819,10 +19813,10 @@
       <c r="AD167" t="s">
         <v>778</v>
       </c>
-      <c r="AE167">
-        <v>1</v>
-      </c>
-      <c r="AF167">
+      <c r="AE167" t="s">
+        <v>1049</v>
+      </c>
+      <c r="AF167" s="2">
         <v>3</v>
       </c>
       <c r="AG167" t="s">
@@ -19938,10 +19932,10 @@
       <c r="AD168" t="s">
         <v>793</v>
       </c>
-      <c r="AE168">
-        <v>1</v>
-      </c>
-      <c r="AF168">
+      <c r="AE168" t="s">
+        <v>1049</v>
+      </c>
+      <c r="AF168" s="2">
         <v>3</v>
       </c>
       <c r="AG168" t="s">
@@ -20057,10 +20051,10 @@
       <c r="AD169" t="s">
         <v>867</v>
       </c>
-      <c r="AE169">
-        <v>1</v>
-      </c>
-      <c r="AF169">
+      <c r="AE169" t="s">
+        <v>1050</v>
+      </c>
+      <c r="AF169" s="2">
         <v>3</v>
       </c>
       <c r="AG169" t="s">
@@ -20551,8 +20545,8 @@
       <c r="AD173" t="s">
         <v>549</v>
       </c>
-      <c r="AE173">
-        <v>1</v>
+      <c r="AE173" t="s">
+        <v>1050</v>
       </c>
       <c r="AF173">
         <v>2.8</v>
@@ -20679,8 +20673,8 @@
       <c r="AD174" t="s">
         <v>633</v>
       </c>
-      <c r="AE174">
-        <v>1</v>
+      <c r="AE174" t="s">
+        <v>1050</v>
       </c>
       <c r="AF174">
         <v>2.8</v>
@@ -20807,8 +20801,8 @@
       <c r="AD175" t="s">
         <v>678</v>
       </c>
-      <c r="AE175">
-        <v>1</v>
+      <c r="AE175" t="s">
+        <v>1050</v>
       </c>
       <c r="AF175">
         <v>2.8</v>
@@ -21173,8 +21167,8 @@
       <c r="AD178" t="s">
         <v>937</v>
       </c>
-      <c r="AE178">
-        <v>1</v>
+      <c r="AE178" t="s">
+        <v>1050</v>
       </c>
       <c r="AF178">
         <v>2.8</v>
@@ -28152,7 +28146,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AQ293">
+  <autoFilter ref="A1:AQ293" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState ref="A2:AQ293">
       <sortCondition descending="1" ref="AF1:AF293"/>
     </sortState>

</xml_diff>